<commit_message>
added to burndown chart
</commit_message>
<xml_diff>
--- a/Scrum/phase 1/Sprint 1/Burndown chart.xlsx
+++ b/Scrum/phase 1/Sprint 1/Burndown chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\ES\ES_gantProject\Scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letic\IdeaProjects\ES_gantProject\Scrum\phase 1\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0612F20-42FD-4196-AB90-DD26581D5538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2CA24C-DD81-4523-8EA5-B936E87CC238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -602,9 +602,40 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -625,37 +656,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,7 +810,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -959,16 +959,16 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2259,102 +2259,102 @@
   <dimension ref="B1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="15" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="46" t="s">
+    <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:20" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="48"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="38"/>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="33">
         <v>44845</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="33">
         <v>44846</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="33">
         <v>44847</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="33">
         <v>44848</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="33">
         <v>44849</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="33">
         <v>44850</v>
       </c>
-      <c r="K4" s="43">
+      <c r="K4" s="33">
         <v>44851</v>
       </c>
-      <c r="L4" s="43">
+      <c r="L4" s="33">
         <v>44852</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="33">
         <v>44853</v>
       </c>
-      <c r="N4" s="43">
+      <c r="N4" s="33">
         <v>44854</v>
       </c>
-      <c r="O4" s="45">
+      <c r="O4" s="34">
         <v>44855</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="32"/>
-      <c r="C5" s="31"/>
+    <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="43"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" s="23">
         <v>1</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="N6" s="7"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" s="25">
         <v>2</v>
       </c>
@@ -2440,11 +2440,11 @@
       <c r="N7" s="10"/>
       <c r="O7" s="11"/>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>3</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="35" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="28">
@@ -2462,7 +2462,7 @@
       <c r="N8" s="10"/>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="25">
         <v>4</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="N9" s="10"/>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="25">
         <v>5</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="N10" s="10"/>
       <c r="O10" s="11"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="25">
         <v>6</v>
       </c>
@@ -2528,7 +2528,7 @@
       <c r="N11" s="10"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="25">
         <v>7</v>
       </c>
@@ -2545,12 +2545,14 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
+      <c r="L12" s="10">
+        <v>1</v>
+      </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="25">
         <v>8</v>
       </c>
@@ -2567,12 +2569,14 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="10">
+        <v>1</v>
+      </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="11"/>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="25">
         <v>9</v>
       </c>
@@ -2594,7 +2598,7 @@
       <c r="N14" s="10"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="25">
         <v>10</v>
       </c>
@@ -2616,119 +2620,119 @@
       <c r="N15" s="10"/>
       <c r="O15" s="11"/>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="37" t="s">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B16" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="3">
         <v>0</v>
       </c>
       <c r="E16" s="16">
-        <f>SUM(E6:E15)</f>
+        <f t="shared" ref="E16:O16" si="0">SUM(E6:E15)</f>
         <v>0</v>
       </c>
       <c r="F16" s="16">
-        <f>SUM(F6:F15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" s="16">
-        <f>SUM(G6:G15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="16">
-        <f>SUM(H6:H15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I16" s="16">
-        <f>SUM(I6:I15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J16" s="16">
-        <f>SUM(J6:J15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K16" s="16">
-        <f>SUM(K6:K15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L16" s="16">
-        <f>SUM(L6:L15)</f>
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M16" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M16" s="16">
-        <f>SUM(M6:M15)</f>
+      <c r="N16" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N16" s="16">
-        <f>SUM(N6:N15)</f>
+      <c r="O16" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O16" s="3">
-        <f>SUM(O6:O15)</f>
-        <v>0</v>
-      </c>
-      <c r="T16" s="39"/>
+      <c r="T16" s="31"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="33" t="s">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="19">
         <f>SUM(D6:D16)</f>
         <v>10</v>
       </c>
       <c r="E17" s="20">
-        <f>D17-SUM(E6:E15)</f>
+        <f t="shared" ref="E17:O17" si="1">D17-SUM(E6:E15)</f>
         <v>10</v>
       </c>
       <c r="F17" s="17">
-        <f>E17-SUM(F6:F15)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G17" s="17">
-        <f>F17-SUM(G6:G15)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="H17" s="17">
-        <f>G17-SUM(H6:H15)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I17" s="17">
-        <f>H17-SUM(I6:I15)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J17" s="15">
-        <f>I17-SUM(J6:J15)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="K17" s="15">
-        <f>J17-SUM(K6:K15)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L17" s="15">
-        <f>K17-SUM(L6:L15)</f>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="M17" s="15">
-        <f>L17-SUM(M6:M15)</f>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="N17" s="17">
-        <f>M17-SUM(N6:N15)</f>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="O17" s="18">
-        <f>N17-SUM(O6:O15)</f>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="35" t="s">
+    <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="21">
         <f>D17</f>
         <v>10</v>
@@ -2780,13 +2784,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B3:O3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update Burndown chart and Sprint Backlog
</commit_message>
<xml_diff>
--- a/Scrum/phase 1/Sprint 1/Burndown chart.xlsx
+++ b/Scrum/phase 1/Sprint 1/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\disnoca\Documents\Universidade\ES\GantProject\ES_gantProject\Scrum\phase 1\Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Faculdade\3ºano\1º Semestre\ES\1ºfase\ES_gantProject\Scrum\phase 1\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C907E2-E000-48DF-979F-A85737251566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095FE1E2-E625-4094-B1A7-31CB6A261443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -610,7 +610,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,6 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -665,7 +665,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,12 +721,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="pt-PT"/>
               <a:t>Sprint Burndown Chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.30645348732276811"/>
+          <c:y val="3.7123213993405513E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -753,7 +760,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -762,25 +769,17 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$16:$C$16</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Completed Effort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -790,10 +789,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$16:$S$16</c:f>
+              <c:f>'Burndown Chart'!$E$16:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -804,10 +803,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -816,18 +815,15 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -835,7 +831,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8D0E-4F8E-897D-5B1720B3868B}"/>
+              <c16:uniqueId val="{00000000-4A50-428F-87F0-959D53617F0B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -847,32 +843,23 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="1048432767"/>
-        <c:axId val="1048433599"/>
+        <c:gapWidth val="219"/>
+        <c:axId val="1616260912"/>
+        <c:axId val="1616258000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$17:$C$17</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Remaining Effort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -883,67 +870,29 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$D$5:$S$5</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Day 0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Day 10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Day 11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$17:$S$17</c:f>
+              <c:f>'Burndown Chart'!$E$17:$O$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0" formatCode="General">
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -953,31 +902,28 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -985,28 +931,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8D0E-4F8E-897D-5B1720B3868B}"/>
+              <c16:uniqueId val="{00000001-4A50-428F-87F0-959D53617F0B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$18:$C$18</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Ideal Burndown</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1015,90 +953,43 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$D$5:$S$5</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Day 0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Day 10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Day 11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$18:$S$18</c:f>
+              <c:f>'Burndown Chart'!$E$18:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>10</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>9.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3333333333333339</c:v>
+                  <c:v>8.6666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.6666666666666661</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3333333333333339</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3333333333333339</c:v>
+                  <c:v>4.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>3.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3333333333333339</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>2.666666666666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -1107,7 +998,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8D0E-4F8E-897D-5B1720B3868B}"/>
+              <c16:uniqueId val="{00000002-4A50-428F-87F0-959D53617F0B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1121,17 +1012,16 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1048432767"/>
-        <c:axId val="1048433599"/>
+        <c:axId val="1616260912"/>
+        <c:axId val="1616258000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1048432767"/>
+        <c:axId val="1616260912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1165,10 +1055,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1048433599"/>
+        <c:crossAx val="1616258000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1176,11 +1066,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1048433599"/>
+        <c:axId val="1616258000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="22"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1198,61 +1086,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Hours</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1281,10 +1114,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1048432767"/>
+        <c:crossAx val="1616260912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1323,7 +1156,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1360,7 +1193,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1412,7 +1245,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1520,11 +1353,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1535,11 +1363,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1571,9 +1394,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1931,23 +1751,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>16807</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180414</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1402878</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114509</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>177054</xdr:rowOff>
+      <xdr:colOff>551721</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9506</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="5" name="Gráfico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D9D4423-6653-CC2E-CA15-1C47386B3EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2265,25 +2085,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:T28"/>
+  <dimension ref="B1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="61" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="15" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:20" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:15" ht="26" x14ac:dyDescent="0.6">
       <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
@@ -2301,7 +2121,7 @@
       <c r="N2" s="41"/>
       <c r="O2" s="42"/>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
@@ -2317,51 +2137,51 @@
       <c r="N3" s="43"/>
       <c r="O3" s="43"/>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="32">
         <v>44845</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <v>44846</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="32">
         <v>44847</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="32">
         <v>44848</v>
       </c>
-      <c r="I4" s="33">
+      <c r="I4" s="32">
         <v>44849</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="32">
         <v>44850</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="32">
         <v>44851</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="32">
         <v>44852</v>
       </c>
-      <c r="M4" s="33">
+      <c r="M4" s="32">
         <v>44853</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="32">
         <v>44854</v>
       </c>
-      <c r="O4" s="34">
+      <c r="O4" s="33">
         <v>44855</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="47"/>
       <c r="C5" s="45"/>
       <c r="D5" s="4" t="s">
@@ -2401,7 +2221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="23">
         <v>1</v>
       </c>
@@ -2425,7 +2245,7 @@
       <c r="N6" s="7"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="25">
         <v>2</v>
       </c>
@@ -2449,11 +2269,11 @@
       <c r="N7" s="10"/>
       <c r="O7" s="11"/>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="25">
         <v>3</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="28">
@@ -2473,7 +2293,7 @@
       <c r="N8" s="10"/>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="25">
         <v>4</v>
       </c>
@@ -2497,7 +2317,7 @@
       <c r="N9" s="10"/>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="25">
         <v>5</v>
       </c>
@@ -2521,7 +2341,7 @@
       <c r="N10" s="10"/>
       <c r="O10" s="11"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="25">
         <v>6</v>
       </c>
@@ -2545,7 +2365,7 @@
       <c r="N11" s="10"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B12" s="25">
         <v>7</v>
       </c>
@@ -2569,7 +2389,7 @@
       <c r="N12" s="10"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B13" s="25">
         <v>8</v>
       </c>
@@ -2593,7 +2413,7 @@
       <c r="N13" s="10"/>
       <c r="O13" s="11"/>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="25">
         <v>9</v>
       </c>
@@ -2610,12 +2430,14 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="L14" s="10">
+        <v>1</v>
+      </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="25">
         <v>10</v>
       </c>
@@ -2632,12 +2454,14 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="L15" s="10">
+        <v>1</v>
+      </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="11"/>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B16" s="38" t="s">
         <v>17</v>
       </c>
@@ -2675,7 +2499,7 @@
       </c>
       <c r="L16" s="16">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M16" s="16">
         <f t="shared" si="0"/>
@@ -2689,9 +2513,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T16" s="31"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="48" t="s">
         <v>16</v>
       </c>
@@ -2730,22 +2553,22 @@
       </c>
       <c r="L17" s="15">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M17" s="15">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N17" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O17" s="18">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="36" t="s">
         <v>18</v>
       </c>
@@ -2799,8 +2622,8 @@
         <v>2.666666666666667</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J28" s="50"/>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="J28" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>